<commit_message>
Tryed positiv Value reading, but the number is negativ with better behaviour, needs fix!!!
</commit_message>
<xml_diff>
--- a/otherinfos/Kalibration/Vergleichswerte.xlsx
+++ b/otherinfos/Kalibration/Vergleichswerte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Repos\Arduino_Project\otherinfos\Kalibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD39B8B-23A8-43F5-A3BF-07E55FECB24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447D0F81-3B97-4DBE-9DEC-934BBD3FD0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="870" windowWidth="14310" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>rawValue</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Theoretische Werte des ADC's</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>7FFFFF</t>
   </si>
 </sst>
 </file>
@@ -101,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -383,16 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -498,7 +510,172 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11101100</v>
+      </c>
+      <c r="B14">
+        <f>LEN(A14)</f>
+        <v>8</v>
+      </c>
+      <c r="C14" t="str">
+        <f>BIN2HEX(A14)</f>
+        <v>EC</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1110011</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:B20" si="0">LEN(A15)</f>
+        <v>7</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" ref="C15:C16" si="1">BIN2HEX(A15)</f>
+        <v>73</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>800000</v>
+      </c>
+      <c r="G15">
+        <f>HEX2DEC(F15)</f>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11101101</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>ED</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <f>HEX2DEC(F17)</f>
+        <v>8388607</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11101100</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C18" t="str">
+        <f>BIN2HEX(A18)</f>
+        <v>EC</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1111010</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" ref="C19:C20" si="2">BIN2HEX(A19)</f>
+        <v>7A</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.11011000111001E+23</v>
+      </c>
+      <c r="I19" t="e">
+        <f>BIN2DEC(H19)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1010000</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11101100</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:B24" si="3">LEN(A22)</f>
+        <v>8</v>
+      </c>
+      <c r="C22" t="str">
+        <f>BIN2HEX(A22)</f>
+        <v>EC</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1010000</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" ref="C23:C24" si="4">BIN2HEX(A23)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>110010</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>